<commit_message>
Prepa release 200-ballot b47dfecd32e0b051d40f413df5c15f0396950344
</commit_message>
<xml_diff>
--- a/336-préparation-publivation-release-200-ballot/ig/CodeSystem-tddui-encounter-identifier.xlsx
+++ b/336-préparation-publivation-release-200-ballot/ig/CodeSystem-tddui-encounter-identifier.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.1.0</t>
+    <t>2.0.0-ballot</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-07-31T15:09:22+00:00</t>
+    <t>2025-07-31T15:41:49+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>